<commit_message>
Manual merge to the latest code from development branch
</commit_message>
<xml_diff>
--- a/application/controllers/AdministratorController.xlsx
+++ b/application/controllers/AdministratorController.xlsx
@@ -15,84 +15,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Stand</t>
   </si>
   <si>
-    <t>Yta</t>
-  </si>
-  <si>
-    <t>Bokad av</t>
-  </si>
-  <si>
-    <t>Erbjuder/Sortiment</t>
-  </si>
-  <si>
-    <t>Tid för bokning</t>
-  </si>
-  <si>
-    <t>Meddelande till arrangör</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>5x5</t>
-  </si>
-  <si>
-    <t>Oneday Wall</t>
-  </si>
-  <si>
-    <t>Click walls</t>
-  </si>
-  <si>
-    <t>17-06-2013 03:29:51</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>2,5x5</t>
-  </si>
-  <si>
-    <t>Multi Trolley</t>
-  </si>
-  <si>
-    <t>Multi Trolleys</t>
-  </si>
-  <si>
-    <t>17-06-2013 06:07:37</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>13x5</t>
-  </si>
-  <si>
-    <t>IT, Wifi</t>
-  </si>
-  <si>
-    <t>07-08-2013 08:47:03</t>
-  </si>
-  <si>
-    <t>clave para el wifi?</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>AerosolTrap</t>
-  </si>
-  <si>
-    <t>Aerosoles y mas</t>
-  </si>
-  <si>
-    <t>14-08-2013 09:18:28</t>
-  </si>
-  <si>
-    <t>Puedes reservarlo?</t>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Booked by</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Time of booking</t>
+  </si>
+  <si>
+    <t>Message to organizer</t>
+  </si>
+  <si>
+    <t>1000-1002</t>
+  </si>
+  <si>
+    <t>9x5m</t>
+  </si>
+  <si>
+    <t>Leif Wallén</t>
+  </si>
+  <si>
+    <t>Plats</t>
+  </si>
+  <si>
+    <t>15-04-2013 13:48:05</t>
+  </si>
+  <si>
+    <t>1713-1715</t>
+  </si>
+  <si>
+    <t>9x5 m</t>
+  </si>
+  <si>
+    <t>Grilltösen</t>
+  </si>
+  <si>
+    <t>Gatuköksprodukter: olika sorters korv, hamburgare, pommes frites</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:28</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>1227-12228</t>
+  </si>
+  <si>
+    <t>6x5 m</t>
+  </si>
+  <si>
+    <t>Nightmare on tour AB</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:37</t>
+  </si>
+  <si>
+    <t>1113-1115</t>
+  </si>
+  <si>
+    <t>Marknadsmedia</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:47</t>
   </si>
 </sst>
 </file>
@@ -525,23 +522,25 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3"/>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -549,22 +548,22 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Konstiga tomma .xlsx-filer som antagligen inte fyller någon funktion.
</commit_message>
<xml_diff>
--- a/application/controllers/AdministratorController.xlsx
+++ b/application/controllers/AdministratorController.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Stand</t>
   </si>
@@ -33,6 +33,63 @@
   </si>
   <si>
     <t>Message to organizer</t>
+  </si>
+  <si>
+    <t>1000-1002</t>
+  </si>
+  <si>
+    <t>9x5m</t>
+  </si>
+  <si>
+    <t>Leif Wallén</t>
+  </si>
+  <si>
+    <t>Plats</t>
+  </si>
+  <si>
+    <t>15-04-2013 13:48:05</t>
+  </si>
+  <si>
+    <t>1713-1715</t>
+  </si>
+  <si>
+    <t>9x5 m</t>
+  </si>
+  <si>
+    <t>Grilltösen</t>
+  </si>
+  <si>
+    <t>Gatuköksprodukter: olika sorters korv, hamburgare, pommes frites</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:28</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>1227-12228</t>
+  </si>
+  <si>
+    <t>6x5 m</t>
+  </si>
+  <si>
+    <t>Nightmare on tour AB</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:37</t>
+  </si>
+  <si>
+    <t>1113-1115</t>
+  </si>
+  <si>
+    <t>Marknadsmedia</t>
+  </si>
+  <si>
+    <t>02-07-2013 08:16:47</t>
   </si>
 </sst>
 </file>
@@ -383,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,6 +488,84 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>